<commit_message>
update 20201006 & 0919/20/21/22
</commit_message>
<xml_diff>
--- a/20200919.xlsx
+++ b/20200919.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EF10AD-092D-4713-8334-C79BE9484947}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16571C3-A067-4C91-8CCA-8ED24BC950A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,7 +186,23 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>2020-09-23 미팅 (금일 제외 D-4)
+    <t>에러 UI 화면 구성</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>인디게이터 마무리</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>에러 UI 연동</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>저녁시간</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-09-23 미팅 (D-4)
 1. UI 완료 (인디게이터 전력계, RFID 연동)
 2. 에러 UI 구성 (에러코드 및 화면 시퀀스 연동)
 3. 타임아웃 적용 (각 시퀀스 별 타임아웃)
@@ -195,29 +211,13 @@
 6. 시간남으면 부트로더 구현</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
-  <si>
-    <t>에러 UI 화면 구성</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>인디게이터 마무리</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>에러 UI 연동</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>저녁시간</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+    <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -934,73 +934,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="1" fillId="32" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="32" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1535,8 +1535,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1551,19 +1551,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>48</v>
       </c>
       <c r="H2" t="s">
@@ -1583,16 +1583,16 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="13" t="s">
-        <v>49</v>
+      <c r="D3" s="4"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="H3" t="s">
         <v>23</v>
@@ -1605,11 +1605,11 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="12"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="19"/>
       <c r="H4" t="s">
         <v>21</v>
       </c>
@@ -1618,11 +1618,11 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="12"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="19"/>
       <c r="H5" t="s">
         <v>22</v>
       </c>
@@ -1631,11 +1631,11 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="12"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="19"/>
       <c r="H6" t="s">
         <v>20</v>
       </c>
@@ -1644,11 +1644,11 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="12"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="19"/>
       <c r="H7" t="s">
         <v>14</v>
       </c>
@@ -1661,11 +1661,11 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="12"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="19"/>
       <c r="H8" t="s">
         <v>6</v>
       </c>
@@ -1674,181 +1674,181 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="12"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="19"/>
       <c r="H9" t="s">
         <v>8</v>
       </c>
       <c r="I9">
         <v>309</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="12"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="12"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="2:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="12"/>
+      <c r="C17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="12"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="2:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="12"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="12"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="12"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="12"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
     </row>
     <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="11"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C24" t="s">

</xml_diff>